<commit_message>
mudança nos arquivos para modelos genéricos
</commit_message>
<xml_diff>
--- a/modelo-dados-teste.xlsx
+++ b/modelo-dados-teste.xlsx
@@ -19,62 +19,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
-  <si>
-    <t>AUXILIAR DE SERVIÇOS GERAIS</t>
-  </si>
-  <si>
-    <t>EMERSON DE FARIA SOARES</t>
-  </si>
-  <si>
-    <t>GERENTE</t>
-  </si>
-  <si>
-    <t>ÉRICA DOS SANTOS MENEZES</t>
-  </si>
-  <si>
-    <t>ANALISTA FINANCEIRO</t>
-  </si>
-  <si>
-    <t>SUBGERENTE</t>
-  </si>
-  <si>
-    <t>WILAMES MELO DA SILVA</t>
-  </si>
-  <si>
-    <t>WILLIAM FREIRE WANG</t>
-  </si>
-  <si>
-    <t>CASA DO AUTISTA</t>
-  </si>
-  <si>
-    <t>CRAS INOÃ</t>
-  </si>
-  <si>
-    <t>MARCELLY LUZIA DE CARVALHO MILIOSI</t>
-  </si>
-  <si>
-    <t>CDA</t>
-  </si>
-  <si>
-    <t>CGR</t>
-  </si>
-  <si>
-    <t>COORDENAÇÃO GERAL DE REABILITAÇÃO</t>
-  </si>
-  <si>
-    <t>CIN</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>MATRÍCULA</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>CARGO</t>
+  </si>
+  <si>
+    <t>SETOR</t>
+  </si>
+  <si>
+    <t>CÓD SETOR</t>
+  </si>
+  <si>
+    <t>NOME1</t>
+  </si>
+  <si>
+    <t>NOME2</t>
+  </si>
+  <si>
+    <t>NOME3</t>
+  </si>
+  <si>
+    <t>NOME4</t>
+  </si>
+  <si>
+    <t>NOME5</t>
+  </si>
+  <si>
+    <t>CARGO1</t>
+  </si>
+  <si>
+    <t>CARGO2</t>
+  </si>
+  <si>
+    <t>CARGO3</t>
+  </si>
+  <si>
+    <t>CARGO4</t>
+  </si>
+  <si>
+    <t>CARGO5</t>
+  </si>
+  <si>
+    <t>SETOR1</t>
+  </si>
+  <si>
+    <t>SETOR2</t>
+  </si>
+  <si>
+    <t>SETOR3</t>
+  </si>
+  <si>
+    <t>SETOR4</t>
+  </si>
+  <si>
+    <t>SETOR5</t>
+  </si>
+  <si>
+    <t>STR1</t>
+  </si>
+  <si>
+    <t>STR2</t>
+  </si>
+  <si>
+    <t>STR3</t>
+  </si>
+  <si>
+    <t>STR4</t>
+  </si>
+  <si>
+    <t>STR5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -144,18 +181,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -369,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L874"/>
+  <dimension ref="A1:L875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -384,106 +424,122 @@
     <col min="5" max="5" width="38.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3">
-        <v>11328</v>
+    <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>11263</v>
+        <v>12345</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>11291</v>
+        <v>12346</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>11329</v>
+        <v>12347</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>11262</v>
+        <v>12348</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>12349</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
+      <c r="D6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1352,6 +1408,7 @@
     <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sortState ref="A2:E970">
     <sortCondition ref="D1"/>

</xml_diff>